<commit_message>
+Churchill (and date handling improvments)
</commit_message>
<xml_diff>
--- a/Allegheny_Municipalities.xlsx
+++ b/Allegheny_Municipalities.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="464">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -260,40 +260,40 @@
     <t xml:space="preserve">http://carnegieborough.com/</t>
   </si>
   <si>
+    <t xml:space="preserve">CASTLE SHANNON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castle Shannon Borough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keystone Oaks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://borough.castle-shannon.pa.us/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHALFANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chalfant Borough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://chalfantborough-pa.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHESWICK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheswick Borough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allegheny Valley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.cheswick.us/</t>
+  </si>
+  <si>
     <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CASTLE SHANNON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Castle Shannon Borough</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keystone Oaks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://borough.castle-shannon.pa.us/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHALFANT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chalfant Borough</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://chalfantborough-pa.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHESWICK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cheswick Borough</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allegheny Valley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.cheswick.us/</t>
   </si>
   <si>
     <t xml:space="preserve">CHURCHILL</t>
@@ -1530,10 +1530,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.85"/>
@@ -1990,24 +1990,24 @@
         <v>20</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>20</v>
@@ -2018,19 +2018,19 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>85</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>59</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>20</v>
@@ -2041,25 +2041,25 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="0" t="s">
+      <c r="D22" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2081,6 +2081,9 @@
       <c r="F23" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="H23" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -2196,7 +2199,7 @@
         <v>115</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>116</v>
@@ -2597,7 +2600,7 @@
         <v>176</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>20</v>
@@ -2640,7 +2643,7 @@
         <v>181</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>154</v>
@@ -3622,7 +3625,7 @@
         <v>309</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F109" s="0" t="s">
         <v>13</v>
@@ -3639,7 +3642,7 @@
         <v>310</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F110" s="0" t="s">
         <v>20</v>
@@ -4079,7 +4082,7 @@
       <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.16"/>

</xml_diff>

<commit_message>
+Ross & 2015 Election Record
</commit_message>
<xml_diff>
--- a/Allegheny_Municipalities.xlsx
+++ b/Allegheny_Municipalities.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="681">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -2251,12 +2251,12 @@
   <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H98" activeCellId="0" sqref="H98"/>
+      <selection pane="bottomLeft" activeCell="H68" activeCellId="0" sqref="H68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.54"/>
@@ -4556,6 +4556,9 @@
       </c>
       <c r="F98" s="0" t="s">
         <v>14</v>
+      </c>
+      <c r="H98" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="I98" s="0" t="s">
         <v>409</v>
@@ -5316,10 +5319,10 @@
   <dimension ref="A1:B86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.42"/>
@@ -5366,10 +5369,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="2" t="n">
         <v>30473</v>
       </c>
     </row>
@@ -6035,7 +6038,7 @@
       <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.16"/>

</xml_diff>

<commit_message>
+Hampton (& Churchill broken)
</commit_message>
<xml_diff>
--- a/Allegheny_Municipalities.xlsx
+++ b/Allegheny_Municipalities.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="681">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -2251,12 +2251,12 @@
   <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H52" activeCellId="0" sqref="H52"/>
+      <selection pane="bottomLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.54"/>
@@ -2872,7 +2872,7 @@
         <v>22</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="I23" s="0" t="s">
         <v>117</v>
@@ -3561,6 +3561,9 @@
       </c>
       <c r="G52" s="0" t="s">
         <v>44</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="I52" s="0" t="s">
         <v>245</v>
@@ -5340,10 +5343,10 @@
   <dimension ref="A1:B86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.42"/>
@@ -5454,10 +5457,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="2" t="n">
         <v>18181</v>
       </c>
     </row>
@@ -6059,7 +6062,7 @@
       <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.16"/>

</xml_diff>

<commit_message>
+Dormont draft (Hampton broken)
</commit_message>
<xml_diff>
--- a/Allegheny_Municipalities.xlsx
+++ b/Allegheny_Municipalities.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="680">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -2250,10 +2250,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+      <selection pane="bottomLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.54"/>
@@ -3026,6 +3026,9 @@
       </c>
       <c r="F29" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>111</v>
       </c>
       <c r="I29" s="0" t="s">
         <v>145</v>
@@ -5346,7 +5349,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.42"/>
@@ -5593,10 +5596,10 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="2" t="n">
         <v>9268</v>
       </c>
     </row>
@@ -5617,34 +5620,34 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="2" t="n">
         <v>8282</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="2" t="n">
         <v>8217</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="2" t="n">
         <v>8216</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="2" t="n">
         <v>8036</v>
       </c>
     </row>
@@ -5657,10 +5660,10 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="2" t="n">
         <v>7806</v>
       </c>
     </row>
@@ -5705,18 +5708,18 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="2" t="n">
         <v>5770</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="2" t="n">
         <v>5424</v>
       </c>
     </row>
@@ -5729,10 +5732,10 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B48" s="2" t="n">
         <v>4903</v>
       </c>
     </row>
@@ -5753,10 +5756,10 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="B51" s="0" t="n">
+      <c r="B51" s="2" t="n">
         <v>4537</v>
       </c>
     </row>
@@ -5833,10 +5836,10 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="B61" s="0" t="n">
+      <c r="B61" s="2" t="n">
         <v>2921</v>
       </c>
     </row>
@@ -5849,18 +5852,18 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B63" s="0" t="n">
+      <c r="B63" s="2" t="n">
         <v>2563</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B64" s="0" t="n">
+      <c r="B64" s="2" t="n">
         <v>2477</v>
       </c>
     </row>
@@ -5905,10 +5908,10 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B70" s="0" t="n">
+      <c r="B70" s="2" t="n">
         <v>1872</v>
       </c>
     </row>
@@ -5921,18 +5924,18 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="B72" s="0" t="n">
+      <c r="B72" s="2" t="n">
         <v>1731</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="B73" s="0" t="n">
+      <c r="B73" s="2" t="n">
         <v>1675</v>
       </c>
     </row>
@@ -5969,10 +5972,10 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="B78" s="0" t="n">
+      <c r="B78" s="2" t="n">
         <v>1388</v>
       </c>
     </row>
@@ -5993,10 +5996,10 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="B81" s="0" t="n">
+      <c r="B81" s="2" t="n">
         <v>1141</v>
       </c>
     </row>
@@ -6033,10 +6036,10 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="A86" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="B86" s="0" t="n">
+      <c r="B86" s="2" t="n">
         <v>363</v>
       </c>
     </row>
@@ -6062,7 +6065,7 @@
       <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.16"/>

</xml_diff>

<commit_message>
Fixed Duquesne and Hampton
</commit_message>
<xml_diff>
--- a/Allegheny_Municipalities.xlsx
+++ b/Allegheny_Municipalities.xlsx
@@ -2248,12 +2248,12 @@
   <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.54"/>
@@ -3077,7 +3077,7 @@
         <v>122</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>111</v>
+        <v>15</v>
       </c>
       <c r="I31" s="0" t="s">
         <v>155</v>
@@ -5349,7 +5349,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.42"/>
@@ -6065,7 +6065,7 @@
       <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.16"/>

</xml_diff>

<commit_message>
+Franklin Park & fixed Pittsburgh
</commit_message>
<xml_diff>
--- a/Allegheny_Municipalities.xlsx
+++ b/Allegheny_Municipalities.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="680">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -2248,12 +2248,12 @@
   <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H46" activeCellId="0" sqref="H46"/>
+      <selection pane="bottomLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.54"/>
@@ -3423,6 +3423,9 @@
       </c>
       <c r="F46" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="I46" s="0" t="s">
         <v>219</v>
@@ -5358,10 +5361,10 @@
   <dimension ref="A1:B86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.42"/>
@@ -5504,10 +5507,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="2" t="n">
         <v>14885</v>
       </c>
     </row>
@@ -6077,7 +6080,7 @@
       <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.16"/>

</xml_diff>

<commit_message>
+West Mifflin and other data
</commit_message>
<xml_diff>
--- a/Allegheny_Municipalities.xlsx
+++ b/Allegheny_Municipalities.xlsx
@@ -10,8 +10,8 @@
   <sheets>
     <sheet name="Spider completion" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Population" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="A-C (pre-Scrapy)" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Home Rule Charters" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Home Rule Charters" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="A-C (pre-Scrapy)" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="824">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -1720,184 +1720,466 @@
     <t xml:space="preserve">wilmerding_b</t>
   </si>
   <si>
-    <t xml:space="preserve">Municipal Entities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population estimates, July 1, 2019,  (V2019)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Municipality of Penn Hills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Municipality of Bethel Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Municipality of Mt. Lebanon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Town of McCandless</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Municipality of Monroeville</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Plum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upper St. Clair Township</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Baldwin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Wilkinsburg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Franklin Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Whitehall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Jefferson Hills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Munhall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Brentwood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O'Hara Township</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Swissvale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Dormont</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Castle Shannon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Bellevue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Pleasant Hills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Carnegie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Oakmont</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Forest Hills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Crafton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Coraopolis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Fox Chapel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Bridgeville</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Green Tree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of North Braddock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Avalon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Tarentum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Glassport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Sewickley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Millvale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Etna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Homestead</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Trafford</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Edgewood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Churchill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Aspinwall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Verona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Emsworth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Wilmerding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of East McKeesport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Rankin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of East Pittsburgh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Ben Avon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Cheswick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Edgeworth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Elizabeth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Blawnox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Whitaker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Leetsdale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Bradford Woods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Lincoln</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Wall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Glen Osborne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borough of Ben Avon Hts</t>
+    <t xml:space="preserve">Municipality </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018 pop. est. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area (miles sq.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pittsburgh city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penn Hills Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mount Lebanon Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bethel Park borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ross Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaler Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">McCandless Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monroeville borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plum borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moon Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Mifflin borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baldwin borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">McKeesport city </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper St. Clair Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hampton Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scott Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilkinsburg borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Fayette Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Fayette Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whitehall borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Franklin Park borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robinson Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Park Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elizabeth Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pine Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Deer Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richland Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munhall borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jefferson Hills borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harrison Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Versailles Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brentwood borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swissvale borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dormont borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O'Hara Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bellevue borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castle Shannon borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pleasant Hills borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carnegie borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Oak borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kennedy Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collier Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indiana Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marshall Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clairton city </t>
+  </si>
+  <si>
+    <t xml:space="preserve">West View borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forest Hills borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oakmont borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilkins Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stowe Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">McKees Rocks borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crafton borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coraopolis borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ohio Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duquesne city </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fox Chapel borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turtle Creek borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Findlay Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bridgeville borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Braddock borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avalon borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarentum borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glassport borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green Tree borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sewickley borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port Vue borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Millvale borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etna borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharpsburg borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Springdale borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mount Oliver borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserve Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingram borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pitcairn borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brackenridge borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trafford borough (comb.) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homestead borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edgewood borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Churchill borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harmar Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aspinwall borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crescent Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liberty borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verona borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emsworth borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fawn Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilmerding borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Braddock borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">McDonald borough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">East McKeesport borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rankin borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baldwin Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Homestead borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aleppo Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Braddock Hills borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Pittsburgh borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dravosburg borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ben Avon borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheswick borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edgeworth borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Springdale Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leet Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versailles borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">East Deer Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elizabeth borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oakdale borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blawnox borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bell Acres borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whitaker borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heidelberg borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leetsdale borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bradford Woods borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frazer Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neville Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lincoln borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sewickley Heights borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chalfant borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kilbuck Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sewickley Hills borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pennsbury Village borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wall borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glen Osborne borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Elizabeth borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thornburg borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosslyn Farms borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ben Avon Heights borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Versailles Township </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glenfield borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haysville borough </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ecode360.com/15796955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bethelpark.net/home-rule-charter/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ecode360.com/12318866</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ecode360.com/29701914</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ecode360.com/14036648</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ecode360.com/26919344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ecode360.com/35347869</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ecode360.com/11766997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mtlebanon.org/2020/Code-Book-and-Home-Rule-Charter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pennhills.org/administration/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ecode360.com/13400768</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://library.municode.com/pa/pittsburgh/codes/code_of_ordinances?nodeId=HORUCHPIPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ecode360.com/27297647</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.twpusc.org/comm-dev/township-code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ecode360.com/30854798</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://whitehallboro.org/whitehall-borough-code/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALLEGHENY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allegheny_co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ecode360.com/8453332</t>
   </si>
   <si>
     <t xml:space="preserve">MUNICIPALITY</t>
@@ -2213,15 +2495,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://benavon.com/taxes-utilities/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://ecode360.com/30854798</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://whitehallboro.org/whitehall-borough-code/</t>
   </si>
 </sst>
 </file>
@@ -2412,12 +2685,12 @@
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="H125" activeCellId="0" sqref="H125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.54"/>
@@ -5692,6 +5965,9 @@
       </c>
       <c r="F124" s="0" t="s">
         <v>25</v>
+      </c>
+      <c r="H124" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="I124" s="0" t="s">
         <v>540</v>
@@ -5950,16 +6226,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5969,685 +6246,1438 @@
       <c r="B1" s="0" t="s">
         <v>566</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>567</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>369</v>
+        <v>568</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>300286</v>
+        <v>302571</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>5248.9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>40807</v>
+        <v>42302</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>2185.4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>32345</v>
+        <v>33102</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>5443.5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>32124</v>
+        <v>32374</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>2773.9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>448</v>
+        <v>572</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>30473</v>
+        <v>31132</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>2150.7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>28193</v>
+        <v>28776</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>2576.2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>27720</v>
+        <v>28733</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>1730.6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="B9" s="3" t="n">
-        <v>27380</v>
+        <v>28386</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>1437.6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>27087</v>
+        <v>27395</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>946</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>359</v>
+        <v>577</v>
       </c>
       <c r="B11" s="3" t="n">
-        <v>25437</v>
+        <v>24786</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>1023.5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>573</v>
+        <v>578</v>
       </c>
       <c r="B12" s="3" t="n">
-        <v>19744</v>
+        <v>20284</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>1398.1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
       <c r="B13" s="3" t="n">
-        <v>19554</v>
+        <v>19801</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>3362.4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="B14" s="3" t="n">
-        <v>18181</v>
+      <c r="A14" s="0" t="s">
+        <v>580</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>19686</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>3637.5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>457</v>
+        <v>581</v>
       </c>
       <c r="B15" s="3" t="n">
-        <v>16428</v>
+        <v>19299</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>1964.1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>475</v>
+        <v>582</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>15945</v>
+        <v>18452</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>1138.7</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>575</v>
+        <v>583</v>
       </c>
       <c r="B17" s="3" t="n">
-        <v>15292</v>
+        <v>17017</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>4349.9</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>576</v>
+        <v>584</v>
       </c>
       <c r="B18" s="3" t="n">
-        <v>14885</v>
+        <v>15906</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>7066.2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>382</v>
+        <v>585</v>
       </c>
       <c r="B19" s="3" t="n">
-        <v>14816</v>
+        <v>14920</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>731.8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>445</v>
+        <v>586</v>
       </c>
       <c r="B20" s="3" t="n">
-        <v>13850</v>
+        <v>14058</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>558.2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>411</v>
+        <v>587</v>
       </c>
       <c r="B21" s="3" t="n">
-        <v>13741</v>
+        <v>13938</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>4191.9</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>479</v>
+        <v>588</v>
       </c>
       <c r="B22" s="3" t="n">
-        <v>13628</v>
+        <v>13919</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>1027.6</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>577</v>
+        <v>589</v>
       </c>
       <c r="B23" s="3" t="n">
-        <v>13393</v>
+        <v>13533</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>900.6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>527</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>11986</v>
+      <c r="A24" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>13503</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>1456.6</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>441</v>
+        <v>591</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>11373</v>
+        <v>13292</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>571.3</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>578</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>11101</v>
+      <c r="A26" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="B26" s="3" t="n">
+        <v>11878</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>699.7</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>579</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>11006</v>
+      <c r="A27" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="B27" s="3" t="n">
+        <v>11854</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>410.5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>274</v>
+        <v>594</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>10236</v>
+        <v>11390</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>778.5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>385</v>
+        <v>595</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>9924</v>
+        <v>11380</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>4767.5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>331</v>
+        <v>596</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>9598</v>
+        <v>10990</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>658.8</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
-        <v>580</v>
-      </c>
-      <c r="B31" s="3" t="n">
-        <v>9268</v>
+      <c r="A31" s="0" t="s">
+        <v>597</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>10468</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>1327.6</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>581</v>
+        <v>598</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>8799</v>
+        <v>10203</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>1246.1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>582</v>
-      </c>
-      <c r="B33" s="0" t="n">
-        <v>8647</v>
+      <c r="A33" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>9620</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>6643.6</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="B34" s="3" t="n">
-        <v>8282</v>
+      <c r="A34" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>8967</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>7214</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>136</v>
+        <v>601</v>
       </c>
       <c r="B35" s="3" t="n">
-        <v>8217</v>
+        <v>8577</v>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>11285.5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="B36" s="3" t="n">
-        <v>8216</v>
+      <c r="A36" s="0" t="s">
+        <v>602</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>8443</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>1145.4</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>585</v>
+        <v>603</v>
       </c>
       <c r="B37" s="3" t="n">
-        <v>8036</v>
+        <v>8352</v>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>7437.2</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>586</v>
-      </c>
-      <c r="B38" s="0" t="n">
-        <v>8026</v>
+      <c r="A38" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>8304</v>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>5199.7</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="s">
-        <v>587</v>
-      </c>
-      <c r="B39" s="3" t="n">
-        <v>7806</v>
+      <c r="A39" s="0" t="s">
+        <v>605</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>8288</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>2984.5</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>399</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>6925</v>
+      <c r="A40" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="B40" s="3" t="n">
+        <v>7961</v>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>4923.3</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>588</v>
+        <v>607</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>6541</v>
+        <v>7858</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>1178.3</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>589</v>
+        <v>608</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>6298</v>
+        <v>7805</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>1411.4</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>492</v>
-      </c>
-      <c r="B43" s="0" t="n">
-        <v>6121</v>
+      <c r="A43" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="B43" s="3" t="n">
+        <v>7433</v>
+      </c>
+      <c r="C43" s="3" t="n">
+        <v>533.7</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>220</v>
+        <v>610</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>6023</v>
+        <v>7309</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>416</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="s">
-        <v>590</v>
-      </c>
-      <c r="B45" s="3" t="n">
-        <v>5770</v>
+      <c r="A45" s="0" t="s">
+        <v>611</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>7255</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>469.4</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>591</v>
+        <v>612</v>
       </c>
       <c r="B46" s="3" t="n">
-        <v>5424</v>
+        <v>6767</v>
+      </c>
+      <c r="C46" s="3" t="n">
+        <v>2240</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>592</v>
+        <v>613</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>5076</v>
+        <v>6759</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>6692.1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="s">
-        <v>593</v>
-      </c>
-      <c r="B48" s="3" t="n">
-        <v>4903</v>
+      <c r="A48" s="0" t="s">
+        <v>614</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>6512</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>4163.7</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>594</v>
+        <v>615</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>4832</v>
+        <v>6380</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>3602.5</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>595</v>
+        <v>616</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>4669</v>
+        <v>6358</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>2316.2</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
-        <v>596</v>
-      </c>
-      <c r="B51" s="3" t="n">
-        <v>4537</v>
+      <c r="A51" s="0" t="s">
+        <v>617</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>6350</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>2764.5</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>597</v>
+        <v>618</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>4366</v>
+        <v>6090</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>5437.5</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>598</v>
-      </c>
-      <c r="B53" s="0" t="n">
-        <v>4315</v>
+      <c r="A53" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="B53" s="3" t="n">
+        <v>5949</v>
+      </c>
+      <c r="C53" s="3" t="n">
+        <v>5204.7</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>599</v>
-      </c>
-      <c r="B54" s="0" t="n">
-        <v>3791</v>
+      <c r="A54" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="B54" s="3" t="n">
+        <v>5664</v>
+      </c>
+      <c r="C54" s="3" t="n">
+        <v>3876.8</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>600</v>
+        <v>621</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>3662</v>
+        <v>5609</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>817.9</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>601</v>
-      </c>
-      <c r="B56" s="0" t="n">
-        <v>3308</v>
+      <c r="A56" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="B56" s="3" t="n">
+        <v>5558</v>
+      </c>
+      <c r="C56" s="3" t="n">
+        <v>2729.9</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>602</v>
+        <v>623</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>3149</v>
+        <v>5409</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>686.9</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>603</v>
+        <v>624</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>3039</v>
+        <v>5335</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>5500</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>269</v>
+        <v>625</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>3007</v>
+        <v>5171</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>160.1</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>604</v>
-      </c>
-      <c r="B60" s="0" t="n">
-        <v>3004</v>
+      <c r="A60" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="B60" s="3" t="n">
+        <v>5142</v>
+      </c>
+      <c r="C60" s="3" t="n">
+        <v>4687.3</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="s">
-        <v>605</v>
-      </c>
-      <c r="B61" s="3" t="n">
-        <v>2921</v>
+      <c r="A61" s="0" t="s">
+        <v>627</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>4847</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>3121.1</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>606</v>
-      </c>
-      <c r="B62" s="0" t="n">
-        <v>2693</v>
+      <c r="A62" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="B62" s="3" t="n">
+        <v>4695</v>
+      </c>
+      <c r="C62" s="3" t="n">
+        <v>6794.5</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B63" s="3" t="n">
-        <v>2563</v>
+      <c r="A63" s="0" t="s">
+        <v>629</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>4521</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>3247.8</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B64" s="3" t="n">
-        <v>2477</v>
+      <c r="A64" s="0" t="s">
+        <v>630</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>4470</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>2501.4</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>607</v>
+        <v>631</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>2411</v>
+        <v>4431</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>2135.4</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>608</v>
+        <v>632</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>2350</v>
+        <v>3821</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>3363.6</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>609</v>
+        <v>633</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>2111</v>
+        <v>3790</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>3225.5</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>610</v>
+        <v>634</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>2042</v>
+        <v>3735</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>5508.8</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>611</v>
+        <v>635</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>2027</v>
+        <v>3442</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>4329.6</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B70" s="3" t="n">
-        <v>1872</v>
+      <c r="A70" s="0" t="s">
+        <v>636</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>3440</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>5383.4</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>612</v>
+        <v>637</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>1757</v>
+        <v>3403</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>3110.6</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="3" t="s">
-        <v>613</v>
-      </c>
-      <c r="B72" s="3" t="n">
-        <v>1731</v>
+      <c r="A72" s="0" t="s">
+        <v>638</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>3394</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>9982.4</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3" t="s">
-        <v>614</v>
-      </c>
-      <c r="B73" s="3" t="n">
-        <v>1675</v>
+      <c r="A73" s="0" t="s">
+        <v>639</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>3375</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>170.3</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>615</v>
+        <v>640</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>1647</v>
+        <v>3331</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>1616.2</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>487</v>
-      </c>
-      <c r="B75" s="0" t="n">
-        <v>1583</v>
+      <c r="A75" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="B75" s="3" t="n">
+        <v>3322</v>
+      </c>
+      <c r="C75" s="3" t="n">
+        <v>7654.4</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>319</v>
+        <v>642</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>1580</v>
+        <v>3286</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>6506.9</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>616</v>
-      </c>
-      <c r="B77" s="0" t="n">
-        <v>1476</v>
+      <c r="A77" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="B77" s="3" t="n">
+        <v>3252</v>
+      </c>
+      <c r="C77" s="3" t="n">
+        <v>5848.9</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3" t="s">
-        <v>617</v>
-      </c>
-      <c r="B78" s="3" t="n">
-        <v>1388</v>
+      <c r="A78" s="0" t="s">
+        <v>644</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>3202</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>2234.5</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>618</v>
+        <v>645</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>1235</v>
+        <v>3155</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>4899.1</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>619</v>
+        <v>646</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>1157</v>
+        <v>3110</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>5298.1</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>620</v>
+        <v>647</v>
       </c>
       <c r="B81" s="3" t="n">
-        <v>1141</v>
+        <v>3008</v>
+      </c>
+      <c r="C81" s="3" t="n">
+        <v>1375.4</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>621</v>
+        <v>648</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>1022</v>
+        <v>2985</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>471.5</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="B83" s="0" t="n">
-        <v>719</v>
+      <c r="A83" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="B83" s="3" t="n">
+        <v>2797</v>
+      </c>
+      <c r="C83" s="3" t="n">
+        <v>7283.9</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
-        <v>622</v>
-      </c>
-      <c r="B84" s="0" t="n">
-        <v>557</v>
+      <c r="A84" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="B84" s="3" t="n">
+        <v>2642</v>
+      </c>
+      <c r="C84" s="3" t="n">
+        <v>1144.7</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>623</v>
+        <v>651</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>538</v>
+        <v>2549</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>1715.3</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3" t="s">
-        <v>624</v>
-      </c>
-      <c r="B86" s="3" t="n">
-        <v>363</v>
+      <c r="A86" s="0" t="s">
+        <v>652</v>
+      </c>
+      <c r="B86" s="0" t="n">
+        <v>2469</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>4142.6</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>653</v>
+      </c>
+      <c r="B87" s="0" t="n">
+        <v>2447</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>3536.1</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>654</v>
+      </c>
+      <c r="B88" s="0" t="n">
+        <v>2379</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>183.7</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>655</v>
+      </c>
+      <c r="B89" s="0" t="n">
+        <v>2185</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>5105.1</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="B90" s="3" t="n">
+        <v>2153</v>
+      </c>
+      <c r="C90" s="3" t="n">
+        <v>3332.8</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>657</v>
+      </c>
+      <c r="B91" s="0" t="n">
+        <v>2135</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>4090</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="B92" s="3" t="n">
+        <v>2132</v>
+      </c>
+      <c r="C92" s="3" t="n">
+        <v>5162.2</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>659</v>
+      </c>
+      <c r="B93" s="0" t="n">
+        <v>2119</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>4212.7</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="B94" s="3" t="n">
+        <v>1986</v>
+      </c>
+      <c r="C94" s="3" t="n">
+        <v>3924.9</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>661</v>
+      </c>
+      <c r="B95" s="0" t="n">
+        <v>1937</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>1912.1</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="B96" s="3" t="n">
+        <v>1917</v>
+      </c>
+      <c r="C96" s="3" t="n">
+        <v>1081.8</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="B97" s="3" t="n">
+        <v>1877</v>
+      </c>
+      <c r="C97" s="3" t="n">
+        <v>1963.4</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="B98" s="0" t="n">
+        <v>1819</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>4688.1</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="B99" s="3" t="n">
+        <v>1785</v>
+      </c>
+      <c r="C99" s="3" t="n">
+        <v>1679.2</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="B100" s="3" t="n">
+        <v>1775</v>
+      </c>
+      <c r="C100" s="3" t="n">
+        <v>3875.5</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="B101" s="3" t="n">
+        <v>1741</v>
+      </c>
+      <c r="C101" s="3" t="n">
+        <v>3171.2</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="B102" s="0" t="n">
+        <v>1681</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>669</v>
+      </c>
+      <c r="B103" s="0" t="n">
+        <v>1635</v>
+      </c>
+      <c r="C103" s="0" t="n">
+        <v>680.1</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>670</v>
+      </c>
+      <c r="B104" s="0" t="n">
+        <v>1632</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <v>1087.3</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>671</v>
+      </c>
+      <c r="B105" s="0" t="n">
+        <v>1510</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <v>2811.9</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B106" s="3" t="n">
+        <v>1495</v>
+      </c>
+      <c r="C106" s="3" t="n">
+        <v>591.8</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>673</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>1488</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>3594.2</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>674</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <v>1457</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>3106.6</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="B109" s="3" t="n">
+        <v>1433</v>
+      </c>
+      <c r="C109" s="3" t="n">
+        <v>3249.4</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="B110" s="3" t="n">
+        <v>1400</v>
+      </c>
+      <c r="C110" s="3" t="n">
+        <v>260.9</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>677</v>
+      </c>
+      <c r="B111" s="0" t="n">
+        <v>1271</v>
+      </c>
+      <c r="C111" s="0" t="n">
+        <v>3863.2</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>678</v>
+      </c>
+      <c r="B112" s="0" t="n">
+        <v>1245</v>
+      </c>
+      <c r="C112" s="0" t="n">
+        <v>4399.3</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>679</v>
+      </c>
+      <c r="B113" s="0" t="n">
+        <v>1215</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="B114" s="3" t="n">
+        <v>1177</v>
+      </c>
+      <c r="C114" s="3" t="n">
+        <v>1322.5</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="B115" s="0" t="n">
+        <v>1156</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>123.7</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="B116" s="0" t="n">
+        <v>1081</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="B117" s="0" t="n">
+        <v>1073</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>214.2</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>684</v>
+      </c>
+      <c r="B118" s="0" t="n">
+        <v>818</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>112.6</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="B119" s="3" t="n">
+        <v>801</v>
+      </c>
+      <c r="C119" s="3" t="n">
+        <v>5037.7</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>686</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>701</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>687</v>
+      </c>
+      <c r="B121" s="0" t="n">
+        <v>689</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>272.5</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="B122" s="3" t="n">
+        <v>668</v>
+      </c>
+      <c r="C122" s="3" t="n">
+        <v>8789.5</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>689</v>
+      </c>
+      <c r="B123" s="0" t="n">
+        <v>579</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>1321.9</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="B124" s="0" t="n">
+        <v>545</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="B125" s="0" t="n">
+        <v>516</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>2089.1</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="B126" s="0" t="n">
+        <v>453</v>
+      </c>
+      <c r="C126" s="0" t="n">
+        <v>1043.8</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>693</v>
+      </c>
+      <c r="B127" s="0" t="n">
+        <v>424</v>
+      </c>
+      <c r="C127" s="0" t="n">
+        <v>755.8</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="B128" s="3" t="n">
+        <v>373</v>
+      </c>
+      <c r="C128" s="3" t="n">
+        <v>2156.1</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>695</v>
+      </c>
+      <c r="B129" s="0" t="n">
+        <v>348</v>
+      </c>
+      <c r="C129" s="0" t="n">
+        <v>358.8</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>696</v>
+      </c>
+      <c r="B130" s="0" t="n">
+        <v>215</v>
+      </c>
+      <c r="C130" s="0" t="n">
+        <v>217.6</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>697</v>
+      </c>
+      <c r="B131" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C131" s="0" t="n">
+        <v>300.4</v>
       </c>
     </row>
   </sheetData>
@@ -6666,13 +7696,405 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.24"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>552</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>715</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>716</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>717</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>718</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.16"/>
@@ -6683,34 +8105,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>625</v>
+        <v>719</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>626</v>
+        <v>720</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>627</v>
+        <v>721</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>628</v>
+        <v>722</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>629</v>
+        <v>723</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>630</v>
+        <v>724</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>631</v>
+        <v>725</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>632</v>
+        <v>726</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6721,13 +8143,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>633</v>
+        <v>727</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>635</v>
+        <v>729</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>2017</v>
@@ -6736,10 +8158,10 @@
         <v>44561</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>637</v>
+        <v>731</v>
       </c>
       <c r="J2" s="4" t="n">
         <v>44100</v>
@@ -6747,13 +8169,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>633</v>
+        <v>727</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>638</v>
+        <v>732</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>2019</v>
@@ -6762,18 +8184,18 @@
         <v>45291</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>639</v>
+        <v>733</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>633</v>
+        <v>727</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>640</v>
+        <v>734</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>2017</v>
@@ -6782,18 +8204,18 @@
         <v>44561</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>633</v>
+        <v>727</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>641</v>
+        <v>735</v>
       </c>
       <c r="G5" s="4" t="n">
         <v>44561</v>
@@ -6801,13 +8223,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>633</v>
+        <v>727</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>642</v>
+        <v>736</v>
       </c>
       <c r="G6" s="4" t="n">
         <v>44561</v>
@@ -6815,19 +8237,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>643</v>
+        <v>737</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>644</v>
+        <v>738</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6838,172 +8260,172 @@
         <v>21</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>645</v>
+        <v>739</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>646</v>
+        <v>740</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>647</v>
+        <v>741</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>649</v>
+        <v>743</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>650</v>
+        <v>744</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>652</v>
+        <v>746</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>653</v>
+        <v>747</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>654</v>
+        <v>748</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>655</v>
+        <v>749</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>656</v>
+        <v>750</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>657</v>
+        <v>751</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>643</v>
+        <v>737</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>658</v>
+        <v>752</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>659</v>
+        <v>753</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7014,168 +8436,168 @@
         <v>21</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>645</v>
+        <v>739</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>660</v>
+        <v>754</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>661</v>
+        <v>755</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>662</v>
+        <v>756</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>663</v>
+        <v>757</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>662</v>
+        <v>756</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>664</v>
+        <v>758</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>662</v>
+        <v>756</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>665</v>
+        <v>759</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>666</v>
+        <v>760</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>667</v>
+        <v>761</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>666</v>
+        <v>760</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>668</v>
+        <v>762</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>666</v>
+        <v>760</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>669</v>
+        <v>763</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>670</v>
+        <v>764</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>671</v>
+        <v>765</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>670</v>
+        <v>764</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>672</v>
+        <v>766</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>670</v>
+        <v>764</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>673</v>
+        <v>767</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>643</v>
+        <v>737</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>674</v>
+        <v>768</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7186,95 +8608,95 @@
         <v>12</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>633</v>
+        <v>727</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>675</v>
+        <v>769</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>676</v>
+        <v>770</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>633</v>
+        <v>727</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>677</v>
+        <v>771</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>633</v>
+        <v>727</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>678</v>
+        <v>772</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>633</v>
+        <v>727</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>679</v>
+        <v>773</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>633</v>
+        <v>727</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>680</v>
+        <v>774</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>643</v>
+        <v>737</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>681</v>
+        <v>775</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7285,161 +8707,161 @@
         <v>21</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>645</v>
+        <v>739</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>682</v>
+        <v>776</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>683</v>
+        <v>777</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>684</v>
+        <v>778</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>639</v>
+        <v>733</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>685</v>
+        <v>779</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>686</v>
+        <v>780</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>687</v>
+        <v>781</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>688</v>
+        <v>782</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>689</v>
+        <v>783</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>639</v>
+        <v>733</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>690</v>
+        <v>784</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>639</v>
+        <v>733</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
-        <v>643</v>
+        <v>737</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>691</v>
+        <v>785</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>639</v>
+        <v>733</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>692</v>
+        <v>786</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7450,161 +8872,161 @@
         <v>21</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>645</v>
+        <v>739</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>693</v>
+        <v>787</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>694</v>
+        <v>788</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>695</v>
+        <v>789</v>
       </c>
       <c r="F45" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>696</v>
+        <v>790</v>
       </c>
       <c r="F46" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>697</v>
+        <v>791</v>
       </c>
       <c r="F47" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>698</v>
+        <v>792</v>
       </c>
       <c r="F48" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>699</v>
+        <v>793</v>
       </c>
       <c r="F49" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>700</v>
+        <v>794</v>
       </c>
       <c r="F50" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>701</v>
+        <v>795</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>643</v>
+        <v>737</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>702</v>
+        <v>796</v>
       </c>
       <c r="F52" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>636</v>
+        <v>730</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>703</v>
+        <v>797</v>
       </c>
       <c r="J52" s="4" t="n">
         <v>44101</v>
@@ -7618,226 +9040,226 @@
         <v>21</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>645</v>
+        <v>739</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>704</v>
+        <v>798</v>
       </c>
       <c r="F53" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>705</v>
+        <v>799</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>662</v>
+        <v>756</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>706</v>
+        <v>800</v>
       </c>
       <c r="F54" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>662</v>
+        <v>756</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>707</v>
+        <v>801</v>
       </c>
       <c r="F55" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>662</v>
+        <v>756</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>708</v>
+        <v>802</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>666</v>
+        <v>760</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>709</v>
+        <v>803</v>
       </c>
       <c r="F57" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>666</v>
+        <v>760</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>710</v>
+        <v>804</v>
       </c>
       <c r="F58" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>666</v>
+        <v>760</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>711</v>
+        <v>805</v>
       </c>
       <c r="F59" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>639</v>
+        <v>733</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>670</v>
+        <v>764</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>712</v>
+        <v>806</v>
       </c>
       <c r="F60" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>670</v>
+        <v>764</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>713</v>
+        <v>807</v>
       </c>
       <c r="F61" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>670</v>
+        <v>764</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>714</v>
+        <v>808</v>
       </c>
       <c r="F62" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>643</v>
+        <v>737</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>715</v>
+        <v>809</v>
       </c>
       <c r="F63" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>639</v>
+        <v>733</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>716</v>
+        <v>810</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>717</v>
+        <v>811</v>
       </c>
       <c r="F64" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="0" t="s">
-        <v>716</v>
+        <v>810</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>718</v>
+        <v>812</v>
       </c>
       <c r="F65" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7848,155 +9270,155 @@
         <v>21</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>645</v>
+        <v>739</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>719</v>
+        <v>813</v>
       </c>
       <c r="F66" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>720</v>
+        <v>814</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>721</v>
+        <v>815</v>
       </c>
       <c r="F67" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>722</v>
+        <v>816</v>
       </c>
       <c r="F68" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>723</v>
+        <v>817</v>
       </c>
       <c r="F69" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>724</v>
+        <v>818</v>
       </c>
       <c r="F70" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>725</v>
+        <v>819</v>
       </c>
       <c r="F71" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>726</v>
+        <v>820</v>
       </c>
       <c r="F72" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="s">
-        <v>648</v>
+        <v>742</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>727</v>
+        <v>821</v>
       </c>
       <c r="F73" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>651</v>
+        <v>745</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>643</v>
+        <v>737</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>634</v>
+        <v>728</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>728</v>
+        <v>822</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>729</v>
+        <v>823</v>
       </c>
     </row>
   </sheetData>
@@ -8017,337 +9439,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.24"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>361</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>387</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>402</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>418</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>440</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>511</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>526</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>528</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>550</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>552</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>732</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
+Jefferson Hills (and fixed Elizabeth Twp)
</commit_message>
<xml_diff>
--- a/Allegheny_Municipalities.xlsx
+++ b/Allegheny_Municipalities.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="824">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -2685,12 +2685,12 @@
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H113" activeCellId="0" sqref="H113"/>
+      <selection pane="bottomLeft" activeCell="H54" activeCellId="0" sqref="H54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.54"/>
@@ -4391,6 +4391,9 @@
       </c>
       <c r="F60" s="0" t="s">
         <v>25</v>
+      </c>
+      <c r="H60" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="I60" s="0" t="s">
         <v>307</v>
@@ -6247,10 +6250,10 @@
   <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
@@ -6578,13 +6581,13 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="3" t="s">
         <v>596</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="3" t="n">
         <v>10990</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="3" t="n">
         <v>658.8</v>
       </c>
     </row>
@@ -7721,7 +7724,7 @@
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.85"/>
@@ -8113,7 +8116,7 @@
       <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.16"/>

</xml_diff>

<commit_message>
+Homestead (& updated Churchill)
</commit_message>
<xml_diff>
--- a/Allegheny_Municipalities.xlsx
+++ b/Allegheny_Municipalities.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="824">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -2685,12 +2685,12 @@
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="H127" activeCellId="0" sqref="H127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.54"/>
@@ -4310,6 +4310,9 @@
       </c>
       <c r="F57" s="0" t="s">
         <v>25</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>121</v>
       </c>
       <c r="I57" s="0" t="s">
         <v>290</v>
@@ -6258,11 +6261,11 @@
   </sheetPr>
   <dimension ref="A1:C131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
@@ -7129,13 +7132,13 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="B79" s="0" t="n">
+      <c r="B79" s="3" t="n">
         <v>3155</v>
       </c>
-      <c r="C79" s="0" t="n">
+      <c r="C79" s="3" t="n">
         <v>4899.1</v>
       </c>
     </row>
@@ -7733,10 +7736,9 @@
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.24"/>
   </cols>
@@ -8125,7 +8127,7 @@
       <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.16"/>

</xml_diff>